<commit_message>
update python and libraries
</commit_message>
<xml_diff>
--- a/examples/awg_measure_wave_gap/wave_gap_calc.xlsx
+++ b/examples/awg_measure_wave_gap/wave_gap_calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\document\e-trees\Q-LEAP\rftool\git\rftool_client\examples\awg_measure_wave_gap\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\document\e-trees\Q-LEAP\rftool\git_new\rftool_client\examples\awg_measure_wave_gap\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C2018B-34B1-4A0C-81BD-CB3ADBFB2B56}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9E510E6-7467-4588-A926-CE3A2AF5B9D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-1710" windowWidth="38640" windowHeight="21390" xr2:uid="{8C371CAD-F185-4982-BEEA-2AE8C75029AF}"/>
+    <workbookView xWindow="5490" yWindow="165" windowWidth="28050" windowHeight="19530" activeTab="1" xr2:uid="{8C371CAD-F185-4982-BEEA-2AE8C75029AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Real (Non-MTS)" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="20">
   <si>
     <t>ステップ</t>
     <phoneticPr fontId="1"/>
@@ -203,13 +203,6 @@
     </rPh>
     <rPh sb="7" eb="9">
       <t>カクホ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Msps  (固定)</t>
-    <rPh sb="7" eb="9">
-      <t>コテイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -428,7 +421,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -450,7 +443,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
@@ -472,12 +465,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1964,7 +1951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D7446C-3058-4BFC-87E6-90F6ABA72E46}">
   <dimension ref="B3:R40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -1985,33 +1972,33 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="2">
         <v>2048.125</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="N3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
       <c r="R3">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
       <c r="R4">
         <v>96</v>
       </c>
@@ -2065,7 +2052,7 @@
       <c r="F9" s="6">
         <v>1</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="7">
         <v>0</v>
       </c>
       <c r="I9" s="3">
@@ -3179,8 +3166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60AEE8D8-B1DD-4044-A64B-FB9B9897352F}">
   <dimension ref="B3:R40"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -3200,33 +3187,33 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="17"/>
-      <c r="D3" s="16">
+      <c r="C3" s="15"/>
+      <c r="D3" s="2">
         <v>3932.16</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="O3" s="17"/>
-      <c r="P3" s="17"/>
-      <c r="Q3" s="17"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15"/>
       <c r="R3">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.4">
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
       <c r="R4">
         <v>96</v>
       </c>
@@ -3280,7 +3267,7 @@
       <c r="F9" s="6">
         <v>1</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="7">
         <v>0</v>
       </c>
       <c r="I9" s="3">
@@ -3360,7 +3347,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="3">
-        <f t="shared" ref="I11:I40" si="3">1000*(N11-K11)/$D$3</f>
+        <f>1000*(N11-K11)/$D$3</f>
         <v>0</v>
       </c>
       <c r="K11">
@@ -3372,7 +3359,7 @@
         <v>0</v>
       </c>
       <c r="M11">
-        <f t="shared" ref="M10:M40" si="4">IF(K11=0, 0, IF((K11+L11)&lt;$R$4, 96, K11+L11))</f>
+        <f t="shared" ref="M11:M40" si="3">IF(K11=0, 0, IF((K11+L11)&lt;$R$4, 96, K11+L11))</f>
         <v>128</v>
       </c>
       <c r="N11">
@@ -3392,7 +3379,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="9"/>
       <c r="I12" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="I11:I40" si="4">1000*(N12-K12)/$D$3</f>
         <v>0</v>
       </c>
       <c r="K12">
@@ -3404,7 +3391,7 @@
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N12">
@@ -3442,7 +3429,7 @@
         <v>0</v>
       </c>
       <c r="M13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>98</v>
       </c>
       <c r="N13">
@@ -3468,7 +3455,7 @@
         <v>0</v>
       </c>
       <c r="I14" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>16.276041666666668</v>
       </c>
       <c r="K14">
@@ -3480,7 +3467,7 @@
         <v>0</v>
       </c>
       <c r="M14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="N14">
@@ -3506,7 +3493,7 @@
         <v>0</v>
       </c>
       <c r="I15" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.3750813802083339</v>
       </c>
       <c r="K15">
@@ -3518,7 +3505,7 @@
         <v>0</v>
       </c>
       <c r="M15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>131</v>
       </c>
       <c r="N15">
@@ -3539,7 +3526,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="9"/>
       <c r="I16" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K16">
@@ -3551,7 +3538,7 @@
         <v>0</v>
       </c>
       <c r="M16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N16">
@@ -3571,7 +3558,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="9"/>
       <c r="I17" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K17">
@@ -3583,7 +3570,7 @@
         <v>0</v>
       </c>
       <c r="M17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N17">
@@ -3603,7 +3590,7 @@
       <c r="F18" s="4"/>
       <c r="G18" s="9"/>
       <c r="I18" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K18">
@@ -3615,7 +3602,7 @@
         <v>0</v>
       </c>
       <c r="M18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N18">
@@ -3635,7 +3622,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="9"/>
       <c r="I19" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K19">
@@ -3647,7 +3634,7 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N19">
@@ -3667,7 +3654,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="9"/>
       <c r="I20" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K20">
@@ -3679,7 +3666,7 @@
         <v>0</v>
       </c>
       <c r="M20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N20">
@@ -3699,7 +3686,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="9"/>
       <c r="I21" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K21">
@@ -3711,7 +3698,7 @@
         <v>0</v>
       </c>
       <c r="M21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N21">
@@ -3731,7 +3718,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="9"/>
       <c r="I22" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K22">
@@ -3743,7 +3730,7 @@
         <v>0</v>
       </c>
       <c r="M22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N22">
@@ -3763,7 +3750,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="9"/>
       <c r="I23" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K23">
@@ -3775,7 +3762,7 @@
         <v>0</v>
       </c>
       <c r="M23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N23">
@@ -3795,7 +3782,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="9"/>
       <c r="I24" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K24">
@@ -3807,7 +3794,7 @@
         <v>0</v>
       </c>
       <c r="M24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N24">
@@ -3827,7 +3814,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="9"/>
       <c r="I25" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K25">
@@ -3839,7 +3826,7 @@
         <v>0</v>
       </c>
       <c r="M25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N25">
@@ -3859,7 +3846,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="9"/>
       <c r="I26" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K26">
@@ -3871,7 +3858,7 @@
         <v>0</v>
       </c>
       <c r="M26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N26">
@@ -3891,7 +3878,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="9"/>
       <c r="I27" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K27">
@@ -3903,7 +3890,7 @@
         <v>0</v>
       </c>
       <c r="M27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N27">
@@ -3923,7 +3910,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="9"/>
       <c r="I28" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K28">
@@ -3935,7 +3922,7 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N28">
@@ -3955,7 +3942,7 @@
       <c r="F29" s="4"/>
       <c r="G29" s="9"/>
       <c r="I29" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K29">
@@ -3967,7 +3954,7 @@
         <v>0</v>
       </c>
       <c r="M29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N29">
@@ -3987,7 +3974,7 @@
       <c r="F30" s="4"/>
       <c r="G30" s="9"/>
       <c r="I30" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K30">
@@ -3999,7 +3986,7 @@
         <v>0</v>
       </c>
       <c r="M30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N30">
@@ -4019,7 +4006,7 @@
       <c r="F31" s="4"/>
       <c r="G31" s="9"/>
       <c r="I31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K31">
@@ -4031,7 +4018,7 @@
         <v>0</v>
       </c>
       <c r="M31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N31">
@@ -4051,7 +4038,7 @@
       <c r="F32" s="4"/>
       <c r="G32" s="9"/>
       <c r="I32" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K32">
@@ -4063,7 +4050,7 @@
         <v>0</v>
       </c>
       <c r="M32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N32">
@@ -4083,7 +4070,7 @@
       <c r="F33" s="4"/>
       <c r="G33" s="9"/>
       <c r="I33" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K33">
@@ -4095,7 +4082,7 @@
         <v>0</v>
       </c>
       <c r="M33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N33">
@@ -4115,7 +4102,7 @@
       <c r="F34" s="4"/>
       <c r="G34" s="9"/>
       <c r="I34" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K34">
@@ -4127,7 +4114,7 @@
         <v>0</v>
       </c>
       <c r="M34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N34">
@@ -4147,7 +4134,7 @@
       <c r="F35" s="4"/>
       <c r="G35" s="9"/>
       <c r="I35" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K35">
@@ -4159,7 +4146,7 @@
         <v>0</v>
       </c>
       <c r="M35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N35">
@@ -4179,7 +4166,7 @@
       <c r="F36" s="4"/>
       <c r="G36" s="9"/>
       <c r="I36" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K36">
@@ -4191,7 +4178,7 @@
         <v>0</v>
       </c>
       <c r="M36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N36">
@@ -4211,7 +4198,7 @@
       <c r="F37" s="4"/>
       <c r="G37" s="9"/>
       <c r="I37" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K37">
@@ -4223,7 +4210,7 @@
         <v>0</v>
       </c>
       <c r="M37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N37">
@@ -4243,7 +4230,7 @@
       <c r="F38" s="4"/>
       <c r="G38" s="9"/>
       <c r="I38" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K38">
@@ -4255,7 +4242,7 @@
         <v>0</v>
       </c>
       <c r="M38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N38">
@@ -4275,7 +4262,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="9"/>
       <c r="I39" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K39">
@@ -4287,7 +4274,7 @@
         <v>0</v>
       </c>
       <c r="M39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N39">
@@ -4307,7 +4294,7 @@
       <c r="F40" s="11"/>
       <c r="G40" s="12"/>
       <c r="I40" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="K40">
@@ -4319,7 +4306,7 @@
         <v>0</v>
       </c>
       <c r="M40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="N40">
@@ -4379,9 +4366,12 @@
       <formula>C9="はい"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C9:C40" xr:uid="{7B5B68AA-96BF-495B-AF7D-15D37B2B063A}">
       <formula1>"はい,いいえ"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3" xr:uid="{8AD50B4D-E738-46D0-BC6D-8689901B3E54}">
+      <formula1>"3932.16,614.4"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4415,33 +4405,33 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="17"/>
+      <c r="C3" s="15"/>
       <c r="D3" s="2">
         <v>6554</v>
       </c>
       <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="P3" s="17" t="s">
+      <c r="P3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Q3" s="17"/>
-      <c r="R3" s="17"/>
-      <c r="S3" s="17"/>
+      <c r="Q3" s="15"/>
+      <c r="R3" s="15"/>
+      <c r="S3" s="15"/>
       <c r="T3">
         <v>32</v>
       </c>
     </row>
     <row r="4" spans="2:20" x14ac:dyDescent="0.4">
-      <c r="P4" s="17" t="s">
+      <c r="P4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
       <c r="T4">
         <v>96</v>
       </c>
@@ -5653,12 +5643,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x01010088D2D0BB1B75CD4A8321680FB4F8255E" ma:contentTypeVersion="0" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="197883e78271c5901dbb215c7345c84e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d559c7c9045c4cdcb708662ab7e4d2f1">
     <xsd:element name="properties">
@@ -5772,6 +5756,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -5782,21 +5772,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DAC3820-DBA2-4CE7-8DAF-198B4EB3DA41}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{16341E93-AB0C-4B04-809C-2BD5D2B661AF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5812,6 +5787,21 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2DAC3820-DBA2-4CE7-8DAF-198B4EB3DA41}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D09AB8D-1CEC-4929-822A-C1D254A20381}">
   <ds:schemaRefs>

</xml_diff>